<commit_message>
17.06.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="20">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -78,7 +78,10 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 16.06.19</t>
+    <t>Date: 17.06.19</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -283,38 +286,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -325,6 +301,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -332,9 +338,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -346,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1524,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1608,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1626,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1645,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1664,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1683,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1702,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1719,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1733,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1783,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1844,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1923,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1985,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2003,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2022,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2041,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2060,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2079,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2096,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2110,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2160,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2221,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2253,14 +2256,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2273,24 +2286,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2321,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2387,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2405,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>47</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>17</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>47000</v>
+        <v>17000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2424,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>141</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>60</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>70500</v>
+        <v>30000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2443,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>591</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>392</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>59100</v>
+        <v>39200</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2462,13 +2465,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>8</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2481,11 +2484,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23">
+        <v>135</v>
+      </c>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2498,13 +2503,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21">
-        <v>100</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2514,14 +2517,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>178000</v>
+        <v>89000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2564,58 +2567,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2625,9 +2628,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2714,72 +2717,74 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
-      <c r="A32" s="6"/>
+      <c r="A32" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2794,13 +2799,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>47</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>17</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>47000</v>
+        <v>17000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2813,13 +2818,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>141</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>60</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>70500</v>
+        <v>30000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2832,13 +2837,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>591</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>392</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>59100</v>
+        <v>39200</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2851,13 +2856,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>8</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>2</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2870,11 +2875,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31">
+        <v>135</v>
+      </c>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>2700</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2887,13 +2894,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34">
-        <v>100</v>
-      </c>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2903,14 +2908,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>178000</v>
+        <v>89000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2953,58 +2958,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3014,9 +3019,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3044,28 +3049,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3082,6 +3065,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3112,63 +3117,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3178,10 +3183,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3196,10 +3201,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3215,10 +3220,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3234,10 +3239,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3253,10 +3258,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3272,10 +3277,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3291,8 +3296,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3305,10 +3310,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3355,60 +3360,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3420,11 +3425,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3499,60 +3504,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3561,10 +3566,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3579,10 +3584,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3598,10 +3603,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3617,10 +3622,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3636,10 +3641,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3655,10 +3660,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3674,8 +3679,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3738,60 +3743,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3803,11 +3808,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3835,30 +3840,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3875,6 +3856,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3906,63 +3911,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3972,10 +3977,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3990,10 +3995,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4009,10 +4014,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4028,10 +4033,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4047,8 +4052,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4064,8 +4069,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4081,8 +4086,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4095,10 +4100,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4145,72 +4150,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4285,60 +4290,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4347,10 +4352,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4365,10 +4370,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4384,10 +4389,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4403,10 +4408,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4422,8 +4427,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4439,8 +4444,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4456,8 +4461,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4470,10 +4475,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4520,58 +4525,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4581,11 +4586,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4613,6 +4618,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4625,34 +4658,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
18.06.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -78,10 +78,10 @@
     <t>Date: 23.04.19</t>
   </si>
   <si>
-    <t>Date: 17.06.19</t>
+    <t>\</t>
   </si>
   <si>
-    <t>\</t>
+    <t>Date: 18.06.19</t>
   </si>
 </sst>
 </file>
@@ -286,11 +286,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,36 +328,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -338,6 +335,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,6 +2256,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2268,32 +2294,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2324,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="A4" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>17</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>44</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>17000</v>
+        <v>44000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>60</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>141</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>70500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>392</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>213</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>39200</v>
+        <v>21300</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>2</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21">
+        <v>24</v>
+      </c>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,13 +2484,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
-        <v>135</v>
-      </c>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2503,8 +2501,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2517,14 +2515,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>89000</v>
+        <v>137000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2567,58 +2565,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2628,9 +2626,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2717,74 +2715,74 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="A31" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2799,13 +2797,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>17</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>44</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>17000</v>
+        <v>44000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2818,13 +2816,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>60</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>141</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>70500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2837,13 +2835,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>392</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>213</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>39200</v>
+        <v>21300</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2856,13 +2854,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>2</v>
-      </c>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21">
+        <v>24</v>
+      </c>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>1200</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2875,13 +2873,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31">
-        <v>135</v>
-      </c>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>2700</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2894,8 +2890,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2908,14 +2904,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>89000</v>
+        <v>137000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2958,58 +2954,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3019,9 +3015,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3049,6 +3045,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3065,28 +3083,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3117,63 +3113,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3183,10 +3179,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3201,10 +3197,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3220,10 +3216,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3239,10 +3235,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3258,10 +3254,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3277,10 +3273,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3296,8 +3292,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3310,10 +3306,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3360,60 +3356,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3425,11 +3421,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3504,60 +3500,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3566,10 +3562,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3584,10 +3580,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3603,10 +3599,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3622,10 +3618,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3641,10 +3637,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3660,10 +3656,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3679,8 +3675,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3743,60 +3739,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3808,11 +3804,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3840,6 +3836,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3856,30 +3876,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3911,63 +3907,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3977,10 +3973,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3995,10 +3991,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4014,10 +4010,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4033,10 +4029,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4052,8 +4048,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4069,8 +4065,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4086,8 +4082,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4100,10 +4096,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4150,72 +4146,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4290,60 +4286,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4352,10 +4348,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4370,10 +4366,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4389,10 +4385,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4408,10 +4404,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4427,8 +4423,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4444,8 +4440,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4461,8 +4457,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4475,10 +4471,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4525,58 +4521,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4586,11 +4582,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4618,16 +4614,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4640,24 +4644,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
19.06.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -81,7 +81,7 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 18.06.19</t>
+    <t>Date: 19.06.19</t>
   </si>
 </sst>
 </file>
@@ -286,38 +286,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -328,6 +301,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,9 +338,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,14 +2256,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2276,24 +2286,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2324,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>44</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>22</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>44000</v>
+        <v>22000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>141</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>113</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>70500</v>
+        <v>56500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>213</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>303</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>21300</v>
+        <v>30300</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>24</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>16</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,11 +2484,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23">
+        <v>20</v>
+      </c>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2501,8 +2503,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2515,14 +2517,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>137000</v>
+        <v>110000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2565,58 +2567,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2626,9 +2628,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2715,60 +2717,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2779,10 +2781,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2797,13 +2799,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>44</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>22</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>44000</v>
+        <v>22000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2816,13 +2818,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>141</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>113</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>70500</v>
+        <v>56500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2835,13 +2837,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>213</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>303</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>21300</v>
+        <v>30300</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2854,13 +2856,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>24</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>16</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>1200</v>
+        <v>800</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2873,11 +2875,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31">
+        <v>20</v>
+      </c>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2890,8 +2894,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2904,14 +2908,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>137000</v>
+        <v>110000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2954,58 +2958,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3015,9 +3019,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3045,28 +3049,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3083,6 +3065,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3113,63 +3117,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3179,10 +3183,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3197,10 +3201,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3216,10 +3220,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3235,10 +3239,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3254,10 +3258,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3273,10 +3277,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3292,8 +3296,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3306,10 +3310,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3356,60 +3360,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3421,11 +3425,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3500,60 +3504,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3562,10 +3566,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3580,10 +3584,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3599,10 +3603,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3618,10 +3622,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3637,10 +3641,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3656,10 +3660,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3675,8 +3679,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3739,60 +3743,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3804,11 +3808,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3836,30 +3840,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3876,6 +3856,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3907,63 +3911,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3973,10 +3977,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3991,10 +3995,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4010,10 +4014,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4029,10 +4033,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4048,8 +4052,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4065,8 +4069,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4082,8 +4086,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4096,10 +4100,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4146,72 +4150,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4286,60 +4290,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4348,10 +4352,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4366,10 +4370,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4385,10 +4389,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4404,10 +4408,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4423,8 +4427,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4440,8 +4444,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4457,8 +4461,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4471,10 +4475,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4521,58 +4525,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4582,11 +4586,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4614,6 +4618,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4626,34 +4658,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
20.06.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -81,7 +81,7 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 19.06.19</t>
+    <t>Date: 20.06.19</t>
   </si>
 </sst>
 </file>
@@ -286,11 +286,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,36 +328,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -338,6 +335,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,6 +2256,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2268,32 +2294,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2306,7 +2306,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+      <selection sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2324,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>22</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>14</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>22000</v>
+        <v>14000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>113</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>85</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>56500</v>
+        <v>42500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>303</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>305</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>30300</v>
+        <v>30500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>16</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,13 +2482,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
-        <v>20</v>
-      </c>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2503,8 +2499,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2517,14 +2513,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>110000</v>
+        <v>87000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2567,58 +2563,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2628,9 +2624,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2717,60 +2713,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2781,10 +2777,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2799,13 +2795,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>22</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>14</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>22000</v>
+        <v>14000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2818,13 +2814,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>113</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>85</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>56500</v>
+        <v>42500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2837,13 +2833,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>303</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>305</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>30300</v>
+        <v>30500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2856,13 +2852,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>16</v>
-      </c>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2875,13 +2869,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31">
-        <v>20</v>
-      </c>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2894,8 +2886,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2908,14 +2900,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>110000</v>
+        <v>87000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2958,58 +2950,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3019,9 +3011,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3049,6 +3041,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3065,28 +3079,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3117,63 +3109,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3183,10 +3175,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3201,10 +3193,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3220,10 +3212,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3239,10 +3231,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3258,10 +3250,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3277,10 +3269,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3296,8 +3288,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3310,10 +3302,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3360,60 +3352,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3425,11 +3417,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3504,60 +3496,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3566,10 +3558,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3584,10 +3576,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3603,10 +3595,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3622,10 +3614,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3641,10 +3633,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3660,10 +3652,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3679,8 +3671,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3743,60 +3735,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3808,11 +3800,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3840,6 +3832,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3856,30 +3872,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3911,63 +3903,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3977,10 +3969,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3995,10 +3987,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4014,10 +4006,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4033,10 +4025,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4052,8 +4044,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4069,8 +4061,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4086,8 +4078,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4100,10 +4092,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4150,72 +4142,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4290,60 +4282,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4352,10 +4344,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4370,10 +4362,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4389,10 +4381,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4408,10 +4400,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4427,8 +4419,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4444,8 +4436,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4461,8 +4453,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4475,10 +4467,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4525,58 +4517,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4586,11 +4578,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4618,16 +4610,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4640,24 +4640,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
24.06.19 Today Sales Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -81,7 +81,7 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 22.06.19</t>
+    <t>Date: 24.06.19</t>
   </si>
 </sst>
 </file>
@@ -2409,12 +2409,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="23">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>67000</v>
+        <v>27000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2428,12 +2428,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="23">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>86000</v>
+        <v>43000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2447,12 +2447,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="23">
-        <v>470</v>
+        <v>100</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>47000</v>
+        <v>10000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,11 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>41</v>
-      </c>
+      <c r="E9" s="23"/>
       <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>2050</v>
+        <v>0</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,13 +2482,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
-        <v>134</v>
-      </c>
+      <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>2680</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2503,13 +2499,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23">
-        <v>27</v>
-      </c>
+      <c r="E11" s="23"/>
       <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2526,7 +2520,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>205000</v>
+        <v>80000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2802,12 +2796,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="23">
-        <v>67</v>
+        <v>27</v>
       </c>
       <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>67000</v>
+        <v>27000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2821,12 +2815,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="23">
-        <v>172</v>
+        <v>86</v>
       </c>
       <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>86000</v>
+        <v>43000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2840,12 +2834,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="23">
-        <v>470</v>
+        <v>100</v>
       </c>
       <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>47000</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2858,13 +2852,11 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>41</v>
-      </c>
+      <c r="E36" s="23"/>
       <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>2050</v>
+        <v>0</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2877,13 +2869,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31">
-        <v>134</v>
-      </c>
+      <c r="E37" s="31"/>
       <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>2680</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2896,13 +2886,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31">
-        <v>27</v>
-      </c>
+      <c r="E38" s="31"/>
       <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2919,7 +2907,7 @@
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>205000</v>
+        <v>80000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>

</xml_diff>

<commit_message>
26.06.19 Today Sales last Updated
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -81,7 +81,7 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 25.06.19</t>
+    <t>Date: 26.06.19</t>
   </si>
 </sst>
 </file>
@@ -286,38 +286,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -328,6 +301,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,9 +338,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,14 +2256,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2276,24 +2286,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2324,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>59</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>61</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>59000</v>
+        <v>61000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>224</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>142</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>112000</v>
+        <v>71000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>391</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>250</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>39100</v>
+        <v>25000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>38</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>186</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>1900</v>
+        <v>9300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,11 +2484,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23">
+        <v>185</v>
+      </c>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2501,8 +2503,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2515,14 +2517,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>212000</v>
+        <v>170000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2565,58 +2567,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2626,9 +2628,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2715,60 +2717,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2779,10 +2781,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2797,13 +2799,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>59</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>61</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>59000</v>
+        <v>61000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2816,13 +2818,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>224</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>142</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>112000</v>
+        <v>71000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2835,13 +2837,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>391</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>250</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>39100</v>
+        <v>25000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2854,13 +2856,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>38</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>186</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>1900</v>
+        <v>9300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2873,11 +2875,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31">
+        <v>185</v>
+      </c>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>3700</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2890,8 +2894,8 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2904,14 +2908,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>212000</v>
+        <v>170000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2954,58 +2958,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3015,9 +3019,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3045,28 +3049,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3083,6 +3065,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3113,63 +3117,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3179,10 +3183,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3197,10 +3201,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3216,10 +3220,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3235,10 +3239,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3254,10 +3258,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3273,10 +3277,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3292,8 +3296,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3306,10 +3310,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3356,60 +3360,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3421,11 +3425,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3500,60 +3504,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3562,10 +3566,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3580,10 +3584,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3599,10 +3603,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3618,10 +3622,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3637,10 +3641,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3656,10 +3660,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3675,8 +3679,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3739,60 +3743,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3804,11 +3808,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3836,30 +3840,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3876,6 +3856,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3907,63 +3911,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3973,10 +3977,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3991,10 +3995,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4010,10 +4014,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4029,10 +4033,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4048,8 +4052,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4065,8 +4069,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4082,8 +4086,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4096,10 +4100,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4146,72 +4150,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4286,60 +4290,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4348,10 +4352,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4366,10 +4370,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4385,10 +4389,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4404,10 +4408,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4423,8 +4427,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4440,8 +4444,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4457,8 +4461,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4471,10 +4475,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4521,58 +4525,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4582,11 +4586,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4614,6 +4618,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4626,34 +4658,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
29.06.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -81,7 +81,7 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 27.06.19</t>
+    <t>Date: 29.06.19</t>
   </si>
 </sst>
 </file>
@@ -286,38 +286,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -328,6 +301,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -335,9 +338,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +349,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1549,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1611,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1629,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1648,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1667,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1686,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1705,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1722,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1736,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1786,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1847,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1926,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1988,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2006,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2025,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2044,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2063,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2082,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2099,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2113,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2163,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2224,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,14 +2256,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2276,24 +2286,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
+      <selection sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2324,63 +2324,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2390,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2408,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>34</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>67</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>34000</v>
+        <v>67000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2427,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>122</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>308</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>61000</v>
+        <v>154000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2446,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>509</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>300</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>50900</v>
+        <v>30000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2465,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>54</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>80</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>2700</v>
+        <v>4000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,13 +2484,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
-        <v>70</v>
-      </c>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2503,10 +2501,10 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="23">
         <v>100</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -2519,14 +2517,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>151000</v>
+        <v>256000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2569,58 +2567,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2630,9 +2628,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2719,60 +2717,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2783,10 +2781,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2801,13 +2799,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>34</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>67</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>34000</v>
+        <v>67000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2820,13 +2818,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>122</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>308</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>61000</v>
+        <v>154000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2839,13 +2837,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>509</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>300</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>50900</v>
+        <v>30000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2858,13 +2856,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>54</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>80</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>2700</v>
+        <v>4000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2877,13 +2875,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34">
-        <v>70</v>
-      </c>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2896,10 +2892,10 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34">
+      <c r="E38" s="31">
         <v>100</v>
       </c>
-      <c r="F38" s="34"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>1000</v>
@@ -2912,14 +2908,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>151000</v>
+        <v>256000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2962,58 +2958,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3023,9 +3019,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3053,28 +3049,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3091,6 +3065,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3121,63 +3117,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3187,10 +3183,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3205,10 +3201,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3224,10 +3220,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3243,10 +3239,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3262,10 +3258,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3281,10 +3277,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3300,8 +3296,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3314,10 +3310,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3364,60 +3360,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3429,11 +3425,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3508,60 +3504,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3570,10 +3566,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3588,10 +3584,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3607,10 +3603,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3626,10 +3622,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3645,10 +3641,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3664,10 +3660,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3683,8 +3679,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3747,60 +3743,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3812,11 +3808,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3844,30 +3840,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3884,6 +3856,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3915,63 +3911,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3981,10 +3977,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3999,10 +3995,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4018,10 +4014,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4037,10 +4033,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4056,8 +4052,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4073,8 +4069,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4090,8 +4086,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4104,10 +4100,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4154,72 +4150,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4294,60 +4290,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4356,10 +4352,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4374,10 +4370,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4393,10 +4389,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4412,10 +4408,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4431,8 +4427,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4448,8 +4444,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4465,8 +4461,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4479,10 +4475,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4529,58 +4525,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4590,11 +4586,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4622,6 +4618,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4634,34 +4658,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
30.06.19 Today sales Details
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="21">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -81,7 +81,10 @@
     <t>\</t>
   </si>
   <si>
-    <t>Date: 29.06.19</t>
+    <t>Date: 30.06.19</t>
+  </si>
+  <si>
+    <t>Almas Tonu</t>
   </si>
 </sst>
 </file>
@@ -286,11 +289,38 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -301,36 +331,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -338,6 +338,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -349,11 +352,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1527,7 +1530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1549,60 +1552,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1611,10 +1614,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1629,10 +1632,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>50</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1648,10 +1651,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>16</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1667,10 +1670,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>151</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1686,10 +1689,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>58</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1705,8 +1708,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1722,8 +1725,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1736,10 +1739,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1786,58 +1789,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1847,11 +1850,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1926,60 +1929,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1988,10 +1991,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2006,10 +2009,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>50</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2025,10 +2028,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>116</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2044,10 +2047,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>151</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2063,10 +2066,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="23">
+      <c r="E35" s="21">
         <v>58</v>
       </c>
-      <c r="F35" s="23"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2082,8 +2085,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2099,8 +2102,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2113,10 +2116,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="20"/>
+      <c r="E38" s="29"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2163,58 +2166,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2224,11 +2227,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2256,6 +2259,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2268,32 +2297,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2305,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E30" workbookViewId="0">
-      <selection sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H47" sqref="A1:J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2324,63 +2327,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2390,10 +2393,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2408,13 +2411,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
-        <v>67</v>
-      </c>
-      <c r="F6" s="23"/>
+      <c r="E6" s="21">
+        <v>42</v>
+      </c>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>67000</v>
+        <v>42000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2427,13 +2430,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
-        <v>308</v>
-      </c>
-      <c r="F7" s="23"/>
+      <c r="E7" s="21">
+        <v>368</v>
+      </c>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>154000</v>
+        <v>184000</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2446,13 +2449,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
-        <v>300</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="E8" s="21">
+        <v>450</v>
+      </c>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>45000</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2465,13 +2468,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
-        <v>80</v>
-      </c>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21">
+        <v>246</v>
+      </c>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>12300</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2484,11 +2487,13 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21">
+        <v>75</v>
+      </c>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2501,13 +2506,13 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23">
-        <v>100</v>
-      </c>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21">
+        <v>720</v>
+      </c>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>7200</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2517,14 +2522,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>256000</v>
+        <v>292000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2567,58 +2572,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2628,9 +2635,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2717,60 +2724,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="24" t="s">
+      <c r="A28" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="27"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2781,10 +2788,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="34" t="s">
+      <c r="E32" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="33"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2799,13 +2806,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="23">
-        <v>67</v>
-      </c>
-      <c r="F33" s="23"/>
+      <c r="E33" s="21">
+        <v>42</v>
+      </c>
+      <c r="F33" s="21"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>67000</v>
+        <v>42000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2818,13 +2825,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="23">
-        <v>308</v>
-      </c>
-      <c r="F34" s="23"/>
+      <c r="E34" s="21">
+        <v>368</v>
+      </c>
+      <c r="F34" s="21"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>154000</v>
+        <v>184000</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2837,13 +2844,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="23">
-        <v>300</v>
-      </c>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21">
+        <v>450</v>
+      </c>
+      <c r="F35" s="21"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>45000</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2856,13 +2863,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="23">
-        <v>80</v>
-      </c>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21">
+        <v>246</v>
+      </c>
+      <c r="F36" s="21"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>4000</v>
+        <v>12300</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2875,11 +2882,13 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34">
+        <v>75</v>
+      </c>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2892,13 +2901,13 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="31">
-        <v>100</v>
-      </c>
-      <c r="F38" s="31"/>
+      <c r="E38" s="34">
+        <v>720</v>
+      </c>
+      <c r="F38" s="34"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>7200</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2908,14 +2917,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="32" t="s">
+      <c r="D39" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="33"/>
+      <c r="E39" s="32"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>256000</v>
+        <v>292000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2958,58 +2967,60 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="21"/>
+      <c r="B43" s="30"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="21" t="s">
+      <c r="H43" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
+      <c r="I43" s="30"/>
+      <c r="J43" s="30"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
+      <c r="J45" s="23"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="22"/>
-      <c r="B46" s="22"/>
+      <c r="A46" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="23"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3019,9 +3030,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3049,6 +3060,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3065,28 +3098,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3117,63 +3128,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3183,10 +3194,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3201,10 +3212,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>68</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3220,10 +3231,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>135</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3239,10 +3250,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>53</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3258,10 +3269,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="21">
         <v>2</v>
       </c>
-      <c r="F9" s="23"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3277,10 +3288,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3296,8 +3307,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3310,10 +3321,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3360,60 +3371,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="22"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3425,11 +3436,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3504,60 +3515,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3566,10 +3577,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="34"/>
+      <c r="F31" s="33"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3584,10 +3595,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="31">
+      <c r="E32" s="34">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3603,10 +3614,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E33" s="34">
         <v>135</v>
       </c>
-      <c r="F33" s="31"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3622,10 +3633,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="34">
         <v>53</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3641,10 +3652,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="31">
+      <c r="E35" s="34">
         <v>2</v>
       </c>
-      <c r="F35" s="31"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3660,10 +3671,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="31">
+      <c r="E36" s="34">
         <v>5</v>
       </c>
-      <c r="F36" s="31"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3679,8 +3690,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3743,60 +3754,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22" t="s">
+      <c r="A45" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3808,11 +3819,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3840,6 +3851,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3856,30 +3891,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3911,63 +3922,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3977,10 +3988,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3995,10 +4006,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>44</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4014,10 +4025,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="21">
         <v>118</v>
       </c>
-      <c r="F7" s="23"/>
+      <c r="F7" s="21"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4033,10 +4044,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="21">
         <v>510</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="21"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4052,8 +4063,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4069,8 +4080,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4086,8 +4097,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4100,10 +4111,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4150,72 +4161,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="29" t="s">
+      <c r="H16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="29"/>
-      <c r="B18" s="29"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="30" t="s">
+      <c r="H19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="30"/>
-      <c r="J19" s="30"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="38"/>
-      <c r="B20" s="38"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4290,60 +4301,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="26" t="s">
+      <c r="A29" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4352,10 +4363,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="17"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4370,10 +4381,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="23">
+      <c r="E32" s="21">
         <v>44</v>
       </c>
-      <c r="F32" s="23"/>
+      <c r="F32" s="21"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4389,10 +4400,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="23">
+      <c r="E33" s="21">
         <v>118</v>
       </c>
-      <c r="F33" s="23"/>
+      <c r="F33" s="21"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4408,10 +4419,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="23">
+      <c r="E34" s="21">
         <v>510</v>
       </c>
-      <c r="F34" s="23"/>
+      <c r="F34" s="21"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4427,8 +4438,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4444,8 +4455,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4461,8 +4472,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="23"/>
-      <c r="F37" s="23"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4475,10 +4486,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="39"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4525,58 +4536,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="30"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="21" t="s">
+      <c r="H42" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="22"/>
-      <c r="B43" s="22"/>
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
+      <c r="J43" s="23"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="22"/>
-      <c r="B44" s="22"/>
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="22"/>
-      <c r="I44" s="22"/>
-      <c r="J44" s="22"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="22"/>
-      <c r="B45" s="22"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4586,11 +4597,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4618,16 +4629,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -4640,24 +4659,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
01.06.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/June/Others/Cash.xlsx
+++ b/June/Others/Cash.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="21">
   <si>
     <t>Tulip-2</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Date: 30.06.19</t>
   </si>
   <si>
-    <t>Almas Tonu</t>
+    <t>Date: 01.07.19</t>
   </si>
 </sst>
 </file>
@@ -289,38 +289,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -331,6 +304,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -338,9 +341,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -352,11 +352,11 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1530,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1552,60 +1552,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -1614,10 +1614,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1632,10 +1632,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>50</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -1651,10 +1651,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>16</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -1670,10 +1670,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>151</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -1689,10 +1689,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>58</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -1708,8 +1708,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1725,8 +1725,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1739,10 +1739,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -1789,58 +1789,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -1850,11 +1850,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -1929,60 +1929,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -1991,10 +1991,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2009,10 +2009,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>50</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2028,10 +2028,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>116</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2047,10 +2047,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>151</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2066,10 +2066,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="23">
         <v>58</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2085,8 +2085,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2102,8 +2102,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2116,10 +2116,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="28" t="s">
+      <c r="D38" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="29"/>
+      <c r="E38" s="20"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2166,58 +2166,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2227,11 +2227,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2259,14 +2259,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2279,24 +2289,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2308,8 +2308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H47" sqref="A1:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2327,63 +2327,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="A4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2393,10 +2393,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2411,13 +2411,13 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
-        <v>42</v>
-      </c>
-      <c r="F6" s="21"/>
+      <c r="E6" s="23">
+        <v>59</v>
+      </c>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>42000</v>
+        <v>59000</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -2430,13 +2430,13 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
-        <v>368</v>
-      </c>
-      <c r="F7" s="21"/>
+      <c r="E7" s="23">
+        <v>161</v>
+      </c>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
-        <v>184000</v>
+        <v>80500</v>
       </c>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -2449,13 +2449,13 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
-        <v>450</v>
-      </c>
-      <c r="F8" s="21"/>
+      <c r="E8" s="23">
+        <v>285</v>
+      </c>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
-        <v>45000</v>
+        <v>28500</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -2468,13 +2468,13 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
-        <v>246</v>
-      </c>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23">
+        <v>100</v>
+      </c>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>12300</v>
+        <v>5000</v>
       </c>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -2487,13 +2487,11 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
-        <v>75</v>
-      </c>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -2506,13 +2504,11 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21">
-        <v>720</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>0</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2522,14 +2518,14 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
-        <v>292000</v>
+        <v>173000</v>
       </c>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
@@ -2572,60 +2568,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2635,9 +2629,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2724,60 +2718,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="19" t="s">
+      <c r="A29" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="27" t="s">
+      <c r="A30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="6" t="s">
@@ -2788,10 +2782,10 @@
       <c r="D32" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="33"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="9" t="s">
         <v>5</v>
       </c>
@@ -2806,13 +2800,13 @@
       <c r="D33" s="2">
         <v>1000</v>
       </c>
-      <c r="E33" s="21">
-        <v>42</v>
-      </c>
-      <c r="F33" s="21"/>
+      <c r="E33" s="23">
+        <v>59</v>
+      </c>
+      <c r="F33" s="23"/>
       <c r="G33" s="2">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>42000</v>
+        <v>59000</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
@@ -2825,13 +2819,13 @@
       <c r="D34" s="2">
         <v>500</v>
       </c>
-      <c r="E34" s="21">
-        <v>368</v>
-      </c>
-      <c r="F34" s="21"/>
+      <c r="E34" s="23">
+        <v>161</v>
+      </c>
+      <c r="F34" s="23"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>184000</v>
+        <v>80500</v>
       </c>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
@@ -2844,13 +2838,13 @@
       <c r="D35" s="2">
         <v>100</v>
       </c>
-      <c r="E35" s="21">
-        <v>450</v>
-      </c>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23">
+        <v>285</v>
+      </c>
+      <c r="F35" s="23"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>45000</v>
+        <v>28500</v>
       </c>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
@@ -2863,13 +2857,13 @@
       <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="21">
-        <v>246</v>
-      </c>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23">
+        <v>100</v>
+      </c>
+      <c r="F36" s="23"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>12300</v>
+        <v>5000</v>
       </c>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
@@ -2882,13 +2876,11 @@
       <c r="D37" s="2">
         <v>20</v>
       </c>
-      <c r="E37" s="34">
-        <v>75</v>
-      </c>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f>SUM(D37*E37)</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
@@ -2901,13 +2893,11 @@
       <c r="D38" s="2">
         <v>10</v>
       </c>
-      <c r="E38" s="34">
-        <v>720</v>
-      </c>
-      <c r="F38" s="34"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>7200</v>
+        <v>0</v>
       </c>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
@@ -2917,14 +2907,14 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="31" t="s">
+      <c r="D39" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="32"/>
+      <c r="E39" s="33"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9">
         <f>SUM(G33:G38)</f>
-        <v>292000</v>
+        <v>173000</v>
       </c>
       <c r="H39" s="6"/>
       <c r="I39" s="6"/>
@@ -2967,60 +2957,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="30" t="s">
+      <c r="H43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="30"/>
-      <c r="J43" s="30"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A46" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="23"/>
+      <c r="A46" s="22"/>
+      <c r="B46" s="22"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="23" t="s">
+      <c r="H46" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="30"/>
-      <c r="J46" s="30"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3030,9 +3018,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="26"/>
-      <c r="J47" s="26"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3060,28 +3048,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3098,6 +3064,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3128,63 +3116,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3194,10 +3182,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3212,10 +3200,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>68</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3231,10 +3219,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>135</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3250,10 +3238,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>53</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3269,10 +3257,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3288,10 +3276,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="23">
         <v>5</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3307,8 +3295,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3321,10 +3309,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3371,60 +3359,60 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="35" t="s">
@@ -3436,11 +3424,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -3515,60 +3503,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -3577,10 +3565,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="33"/>
+      <c r="F31" s="34"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -3595,10 +3583,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="31">
         <v>68</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -3614,10 +3602,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="31">
         <v>135</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -3633,10 +3621,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="31">
         <v>53</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -3652,10 +3640,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="31">
         <v>2</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3671,10 +3659,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="34">
+      <c r="E36" s="31">
         <v>5</v>
       </c>
-      <c r="F36" s="34"/>
+      <c r="F36" s="31"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3690,8 +3678,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3754,60 +3742,60 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="23"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36" t="s">
@@ -3819,11 +3807,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3851,30 +3839,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -3891,6 +3855,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -3922,63 +3910,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3988,10 +3976,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="28"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4006,10 +3994,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="23">
         <v>44</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="23"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4025,10 +4013,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="23">
         <v>118</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4044,10 +4032,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="23">
         <v>510</v>
       </c>
-      <c r="F8" s="21"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4063,8 +4051,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4080,8 +4068,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4097,8 +4085,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4111,10 +4099,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="17"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4161,72 +4149,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
+      <c r="A19" s="22"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="30"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4301,60 +4289,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4363,10 +4351,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4381,10 +4369,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="23">
         <v>44</v>
       </c>
-      <c r="F32" s="21"/>
+      <c r="F32" s="23"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4400,10 +4388,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="23">
         <v>118</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="23"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4419,10 +4407,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="23">
         <v>510</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="23"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4438,8 +4426,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4455,8 +4443,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4472,8 +4460,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4486,10 +4474,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="38" t="s">
+      <c r="D38" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="39"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -4536,58 +4524,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="30"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="30" t="s">
+      <c r="H42" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="30"/>
-      <c r="J42" s="30"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
+      <c r="A43" s="22"/>
+      <c r="B43" s="22"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
+      <c r="A44" s="22"/>
+      <c r="B44" s="22"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
+      <c r="A45" s="22"/>
+      <c r="B45" s="22"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="23" t="s">
+      <c r="H45" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="30"/>
-      <c r="J45" s="30"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="36"/>
@@ -4597,11 +4585,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="25" t="s">
+      <c r="H46" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="26"/>
-      <c r="J46" s="26"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4629,6 +4617,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -4641,34 +4657,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>